<commit_message>
anh TO tra 4tr
</commit_message>
<xml_diff>
--- a/TongKetThangAnhTo.xlsx
+++ b/TongKetThangAnhTo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t>Vàng</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>16/10/2024</t>
+  </si>
+  <si>
+    <t>11/01/2025</t>
   </si>
 </sst>
 </file>
@@ -511,12 +514,24 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -526,22 +541,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -992,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="F119" sqref="F119"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="P131" sqref="P131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,14 +1013,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1168,12 +1171,12 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1237,12 +1240,12 @@
       <c r="A19" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="50">
+      <c r="B19" s="54">
         <f>SUM(B18:D18)</f>
         <v>223</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="6"/>
       <c r="F19" s="34"/>
       <c r="G19" s="2"/>
@@ -1285,12 +1288,12 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
+      <c r="A22" s="56"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1392,13 +1395,13 @@
       <c r="A34" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="47">
+      <c r="B34" s="49">
         <f>SUM(B33:E33)</f>
         <v>284</v>
       </c>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="48"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="50"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -1437,13 +1440,13 @@
       <c r="A37" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="57">
+      <c r="B37" s="47">
         <f>SUM(B36:E36)</f>
         <v>840</v>
       </c>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
@@ -1538,10 +1541,10 @@
       <c r="H50" s="24"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="54" t="s">
+      <c r="B51" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="54"/>
+      <c r="C51" s="48"/>
       <c r="E51" s="24"/>
       <c r="H51" s="24"/>
     </row>
@@ -1587,8 +1590,8 @@
       <c r="H55" s="18"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="47"/>
-      <c r="C56" s="48"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="50"/>
       <c r="E56" s="18"/>
       <c r="H56" s="18"/>
     </row>
@@ -1901,7 +1904,12 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="26"/>
-      <c r="B131" s="26"/>
+      <c r="B131" s="26">
+        <v>4000</v>
+      </c>
+      <c r="C131" s="41" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="26"/>
@@ -1932,7 +1940,7 @@
       </c>
       <c r="B138">
         <f>SUM(B126:B136)</f>
-        <v>6000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -1941,7 +1949,7 @@
       </c>
       <c r="B139" s="31">
         <f>B125-B138</f>
-        <v>4580.8950000000004</v>
+        <v>580.89500000000044</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>